<commit_message>
Included some more requirements
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\the-rampage-game\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C116881B-B45A-43C3-BDFD-D1E4F351B057}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC6581-18B2-4769-9154-087C76A911D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{DC5262C6-FF6A-43DC-A405-55288C9DAB63}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Permite al usuario elegir entre dos personajes al inicio del juego. Este será el personaje con el que jugará a través de los diferentes niveles.</t>
   </si>
   <si>
-    <t>Evento de elección</t>
-  </si>
-  <si>
     <t>Archivo de texto a cargar</t>
   </si>
   <si>
@@ -105,6 +102,33 @@
   </si>
   <si>
     <t xml:space="preserve">Se mueve el personaje acorde a la dirección que elige el usuario. </t>
+  </si>
+  <si>
+    <t>Destruir edificio</t>
+  </si>
+  <si>
+    <t>Cuando el personaje golpea al edificio, este empieza a destruirse hasta derrumbarse.</t>
+  </si>
+  <si>
+    <t>Objeto de tipo jugador</t>
+  </si>
+  <si>
+    <t>Coordenadas de ambos objetos que entran en colisión</t>
+  </si>
+  <si>
+    <t>El edificio va desaparece en las coordenadas de colisión.</t>
+  </si>
+  <si>
+    <t>Entrar en bonus</t>
+  </si>
+  <si>
+    <t>Cuando el personaje entra a cierta parte de la escena, cae en un nivel bonus, entrando en otra escena.</t>
+  </si>
+  <si>
+    <t>Coordenadas del objeto y coordenadas a comparar</t>
+  </si>
+  <si>
+    <t>Se cambia la escena, cargando la escena del bonus respectivo.</t>
   </si>
 </sst>
 </file>
@@ -462,7 +486,7 @@
   <dimension ref="D2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +494,7 @@
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
     <col min="6" max="6" width="37.109375" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
     <col min="8" max="8" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,10 +526,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="4:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -516,13 +540,13 @@
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="4:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -530,35 +554,51 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="4:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">

</xml_diff>